<commit_message>
Added default currency formatting.
</commit_message>
<xml_diff>
--- a/docs/type transforms.xlsx
+++ b/docs/type transforms.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="42">
   <si>
     <t>string</t>
   </si>
@@ -69,9 +69,6 @@
     <t>:date</t>
   </si>
   <si>
-    <t>:utc_datetime</t>
-  </si>
-  <si>
     <t>:time</t>
   </si>
   <si>
@@ -130,6 +127,24 @@
   </si>
   <si>
     <t>Assumes ISO 8601 format</t>
+  </si>
+  <si>
+    <t>:datetime</t>
+  </si>
+  <si>
+    <t>DateTime</t>
+  </si>
+  <si>
+    <t>"YYYY-MM-DD hh:mm:ssZ"</t>
+  </si>
+  <si>
+    <t>Assumes integer is unix_time</t>
+  </si>
+  <si>
+    <t>:currency</t>
+  </si>
+  <si>
+    <t>Y (S-&gt;D-&gt;C)</t>
   </si>
 </sst>
 </file>
@@ -191,8 +206,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="41">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -241,7 +264,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="41">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -262,6 +285,10 @@
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -282,6 +309,10 @@
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -611,10 +642,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -624,7 +655,7 @@
     <col min="4" max="4" width="14.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -649,10 +680,13 @@
       <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>12</v>
@@ -666,10 +700,13 @@
       <c r="G2" t="s">
         <v>14</v>
       </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -683,10 +720,13 @@
       <c r="G3" t="s">
         <v>3</v>
       </c>
+      <c r="H3" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" spans="1:9">
       <c r="A4" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -700,10 +740,13 @@
       <c r="G4" t="s">
         <v>3</v>
       </c>
+      <c r="H4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:9">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C5" t="s">
         <v>10</v>
@@ -717,10 +760,13 @@
       <c r="G5" t="s">
         <v>3</v>
       </c>
+      <c r="H5" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
         <v>11</v>
@@ -733,6 +779,9 @@
       </c>
       <c r="F6" t="s">
         <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:9">
@@ -746,13 +795,13 @@
         <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>0</v>
@@ -760,68 +809,70 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" t="s">
         <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="A10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" t="s">
         <v>24</v>
-      </c>
-      <c r="C10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G10" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G11" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:9">
       <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="1"/>
-      <c r="G12" t="s">
-        <v>35</v>
+      <c r="I12" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:9">
@@ -829,24 +880,42 @@
         <v>31</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="D13" t="s">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="E13" t="s">
-        <v>3</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="I13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" t="s">
-        <v>18</v>
+        <v>33</v>
+      </c>
+      <c r="F13" s="1"/>
+      <c r="G13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" t="s">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>